<commit_message>
Updates to Terrestrial and Marine_artificial crosswalks
</commit_message>
<xml_diff>
--- a/crosswalks/Marine-IUCNGET/Marine_artificial-IUCN.xlsx
+++ b/crosswalks/Marine-IUCNGET/Marine_artificial-IUCN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/jor069_csiro_au/Documents/NEAP/ecosystem-typology_working-copies/crosswalks/Marine-IUCNGET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{07831EE1-F4C5-4AA8-ADAA-3317841407F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4C43AF6-8B2F-4A8C-B150-0620BD05D407}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{E92812AE-4504-4A60-8587-C2BDBBD663CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7EF3E71F-E556-48B4-ACB4-0AE5B9E9B6FD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1995" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{34DC40AB-52EF-7A46-B6BC-4735B97204DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{34DC40AB-52EF-7A46-B6BC-4735B97204DB}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="3" r:id="rId1"/>
@@ -90,9 +90,6 @@
     <t>mapping_set_id: http://w3id.org/env/crosswalk/nesp2get/2024-02-06</t>
   </si>
   <si>
-    <t xml:space="preserve">   oil: https://data.imas.utas.edu.au/attachments/NESP_pressures/DATA/Mining/Construction_and_operation_of_pipelines/</t>
-  </si>
-  <si>
     <t xml:space="preserve">   petrol: https://nopta.gov.au/maps-and-public-data/shape-files/PetroleumWells_Jun2024.zip</t>
   </si>
   <si>
@@ -226,15 +223,25 @@
   </si>
   <si>
     <t xml:space="preserve">   cableGA: https://amsis-geoscience-au.hub.arcgis.com/datasets/bc1e7fb37fca40faa5dafbc8a5a4dc3c/explore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   oil: https://data.gov.au/data/dataset/cf647d62-adae-4c92-a430-9706e006eb1f</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -311,18 +318,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -342,33 +343,36 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="17" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,42 +727,42 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -778,7 +782,7 @@
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -828,355 +832,346 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7611E86-6A25-5D4D-8000-7C81AAA55AB6}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.19921875" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.19921875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.8984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.8984375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="30.796875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.19921875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.59765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.59765625" style="10" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.8984375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.59765625" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.296875" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.19921875" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.19921875" style="10"/>
+    <col min="1" max="1" width="21.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.8984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.8984375" style="8" customWidth="1"/>
+    <col min="5" max="5" width="30.796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.59765625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.59765625" style="8" customWidth="1"/>
+    <col min="9" max="9" width="10.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.8984375" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.59765625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31" style="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.19921875" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.19921875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" ht="12" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:15" s="12" customFormat="1" ht="12" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="N1" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="O1" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="I3" s="9">
+        <v>45474</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="6"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="6" t="s">
+      <c r="E4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="10" t="s">
+      <c r="G4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="9">
+        <v>45474</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="6"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="9">
+        <v>45474</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="6"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="9">
+        <v>45474</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="9">
+        <v>45474</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="9">
+        <v>45474</v>
+      </c>
+      <c r="K8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I3" s="12">
-        <v>45474</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="12">
-        <v>45474</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I5" s="12">
-        <v>45474</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I6" s="12">
-        <v>45474</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O6" s="8"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="12">
-        <v>45474</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I8" s="12">
-        <v>45474</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G9" s="17"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G10" s="17"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="G11" s="17"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+      <c r="A20" s="10"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14"/>
+      <c r="A21" s="10"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14"/>
+      <c r="A22" s="10"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14"/>
+      <c r="A23" s="10"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14"/>
+      <c r="A24" s="10"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="13"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A25" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>